<commit_message>
added more dl links for operations
capacity of generation on outage, 2026, January 01-28
</commit_message>
<xml_diff>
--- a/scripts/generate_public_data_archive_commands.xlsx
+++ b/scripts/generate_public_data_archive_commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ecg0122\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99707769-1FB9-4202-BC39-F4E7687284F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5B426D-2C0D-4896-9978-26412D0A6757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4C33C789-5DD0-4FEC-827C-9D753644E8AA}"/>
+    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{4C33C789-5DD0-4FEC-827C-9D753644E8AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="18">
   <si>
     <t>RAMP-UNCERTAINTY</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>PowerShell Command w/ built-in sleep</t>
+  </si>
+  <si>
+    <t>Capacity-Gen-Outage</t>
   </si>
 </sst>
 </file>
@@ -474,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8C02E9D-2D95-4772-99B2-4EA067BBE757}">
-  <dimension ref="A1:AJ25"/>
+  <dimension ref="A1:AJ55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,7 +549,7 @@
         <v>20250201</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G25" si="0">_xlfn.CONCAT("Start-Sleep -Seconds 3;" &amp; " Invoke-WebRequest -Uri" &amp; " '" &amp; AI3 &amp; "'" &amp; " -OutFile " &amp; "'" &amp; AJ3 &amp; "';")</f>
+        <f t="shared" ref="G3:G55" si="0">_xlfn.CONCAT("Start-Sleep -Seconds 3;" &amp; " Invoke-WebRequest -Uri" &amp; " '" &amp; AI3 &amp; "'" &amp; " -OutFile " &amp; "'" &amp; AJ3 &amp; "';")</f>
         <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/ramp-uncertainty?path=%2F2025%2F02%2FRAMP-UNCERTAINTY-20250201.csv' -OutFile 'D:\pub_data_archive\operations\ramp-uncertainty\2025\RAMP-UNCERTAINTY-20250201.csv';</v>
       </c>
       <c r="AI3" t="str">
@@ -554,7 +557,7 @@
         <v>https://portal.spp.org/file-browser-api/download/ramp-uncertainty?path=%2F2025%2F02%2FRAMP-UNCERTAINTY-20250201.csv</v>
       </c>
       <c r="AJ3" t="str">
-        <f t="shared" ref="AJ3:AJ25" si="2">_xlfn.CONCAT("D:\pub_data_archive\" &amp; LOWER(A3) &amp;"\"&amp; LOWER(D3) &amp; "\" &amp; B3&amp;"\" &amp; D3 &amp;"-"&amp;E3&amp;".csv")</f>
+        <f t="shared" ref="AJ3:AJ55" si="2">_xlfn.CONCAT("D:\pub_data_archive\" &amp; LOWER(A3) &amp;"\"&amp; LOWER(D3) &amp; "\" &amp; B3&amp;"\" &amp; D3 &amp;"-"&amp;E3&amp;".csv")</f>
         <v>D:\pub_data_archive\operations\ramp-uncertainty\2025\RAMP-UNCERTAINTY-20250201.csv</v>
       </c>
     </row>
@@ -1194,6 +1197,847 @@
       <c r="AJ25" t="str">
         <f t="shared" si="2"/>
         <v>D:\pub_data_archive\operations\ramp-uncertainty\2024\RAMP-UNCERTAINTY-20241201.csv</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27">
+        <v>2026</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27">
+        <v>20260101</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260101.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260101.csv';</v>
+      </c>
+      <c r="AI27" t="str">
+        <f>_xlfn.CONCAT("https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage" &amp; "?path=%2F" &amp; B27 &amp; "%2F" &amp; C27 &amp; "%2F" &amp; D27 &amp; "-" &amp; E27 &amp; ".csv")</f>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260101.csv</v>
+      </c>
+      <c r="AJ27" t="str">
+        <f>_xlfn.CONCAT("D:\pub_data_archive\" &amp; LOWER(A27) &amp;"\"&amp; LOWER(D27) &amp; "\" &amp; B27&amp;"\" &amp; C27 &amp; "\" &amp; D27 &amp;"-"&amp;E27&amp;".csv")</f>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260101.csv</v>
+      </c>
+    </row>
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28">
+        <v>2026</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28">
+        <v>20260102</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260102.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260102.csv';</v>
+      </c>
+      <c r="AI28" t="str">
+        <f t="shared" ref="AI28:AI55" si="3">_xlfn.CONCAT("https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage" &amp; "?path=%2F" &amp; B28 &amp; "%2F" &amp; C28 &amp; "%2F" &amp; D28 &amp; "-" &amp; E28 &amp; ".csv")</f>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260102.csv</v>
+      </c>
+      <c r="AJ28" t="str">
+        <f t="shared" ref="AJ28:AJ55" si="4">_xlfn.CONCAT("D:\pub_data_archive\" &amp; LOWER(A28) &amp;"\"&amp; LOWER(D28) &amp; "\" &amp; B28&amp;"\" &amp; C28 &amp; "\" &amp; D28 &amp;"-"&amp;E28&amp;".csv")</f>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260102.csv</v>
+      </c>
+    </row>
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29">
+        <v>2026</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29">
+        <v>20260103</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260103.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260103.csv';</v>
+      </c>
+      <c r="AI29" t="str">
+        <f t="shared" si="3"/>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260103.csv</v>
+      </c>
+      <c r="AJ29" t="str">
+        <f t="shared" si="4"/>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260103.csv</v>
+      </c>
+    </row>
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30">
+        <v>2026</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30">
+        <v>20260104</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260104.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260104.csv';</v>
+      </c>
+      <c r="AI30" t="str">
+        <f t="shared" si="3"/>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260104.csv</v>
+      </c>
+      <c r="AJ30" t="str">
+        <f t="shared" si="4"/>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260104.csv</v>
+      </c>
+    </row>
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31">
+        <v>2026</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31">
+        <v>20260105</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260105.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260105.csv';</v>
+      </c>
+      <c r="AI31" t="str">
+        <f t="shared" si="3"/>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260105.csv</v>
+      </c>
+      <c r="AJ31" t="str">
+        <f t="shared" si="4"/>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260105.csv</v>
+      </c>
+    </row>
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32">
+        <v>2026</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32">
+        <v>20260106</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260106.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260106.csv';</v>
+      </c>
+      <c r="AI32" t="str">
+        <f t="shared" si="3"/>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260106.csv</v>
+      </c>
+      <c r="AJ32" t="str">
+        <f t="shared" si="4"/>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260106.csv</v>
+      </c>
+    </row>
+    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33">
+        <v>2026</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33">
+        <v>20260107</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260107.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260107.csv';</v>
+      </c>
+      <c r="AI33" t="str">
+        <f t="shared" si="3"/>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260107.csv</v>
+      </c>
+      <c r="AJ33" t="str">
+        <f t="shared" si="4"/>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260107.csv</v>
+      </c>
+    </row>
+    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34">
+        <v>2026</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34">
+        <v>20260108</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260108.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260108.csv';</v>
+      </c>
+      <c r="AI34" t="str">
+        <f t="shared" si="3"/>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260108.csv</v>
+      </c>
+      <c r="AJ34" t="str">
+        <f t="shared" si="4"/>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260108.csv</v>
+      </c>
+    </row>
+    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35">
+        <v>2026</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35">
+        <v>20260109</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260109.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260109.csv';</v>
+      </c>
+      <c r="AI35" t="str">
+        <f t="shared" si="3"/>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260109.csv</v>
+      </c>
+      <c r="AJ35" t="str">
+        <f t="shared" si="4"/>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260109.csv</v>
+      </c>
+    </row>
+    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36">
+        <v>2026</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36">
+        <v>20260110</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260110.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260110.csv';</v>
+      </c>
+      <c r="AI36" t="str">
+        <f t="shared" si="3"/>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260110.csv</v>
+      </c>
+      <c r="AJ36" t="str">
+        <f t="shared" si="4"/>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260110.csv</v>
+      </c>
+    </row>
+    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37">
+        <v>2026</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37">
+        <v>20260111</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260111.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260111.csv';</v>
+      </c>
+      <c r="AI37" t="str">
+        <f t="shared" si="3"/>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260111.csv</v>
+      </c>
+      <c r="AJ37" t="str">
+        <f t="shared" si="4"/>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260111.csv</v>
+      </c>
+    </row>
+    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38">
+        <v>2026</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38">
+        <v>20260112</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260112.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260112.csv';</v>
+      </c>
+      <c r="AI38" t="str">
+        <f t="shared" si="3"/>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260112.csv</v>
+      </c>
+      <c r="AJ38" t="str">
+        <f t="shared" si="4"/>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260112.csv</v>
+      </c>
+    </row>
+    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39">
+        <v>2026</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39">
+        <v>20260113</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260113.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260113.csv';</v>
+      </c>
+      <c r="AI39" t="str">
+        <f t="shared" si="3"/>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260113.csv</v>
+      </c>
+      <c r="AJ39" t="str">
+        <f t="shared" si="4"/>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260113.csv</v>
+      </c>
+    </row>
+    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40">
+        <v>2026</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40">
+        <v>20260114</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260114.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260114.csv';</v>
+      </c>
+      <c r="AI40" t="str">
+        <f t="shared" si="3"/>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260114.csv</v>
+      </c>
+      <c r="AJ40" t="str">
+        <f t="shared" si="4"/>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260114.csv</v>
+      </c>
+    </row>
+    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41">
+        <v>2026</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41">
+        <v>20260115</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260115.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260115.csv';</v>
+      </c>
+      <c r="AI41" t="str">
+        <f t="shared" si="3"/>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260115.csv</v>
+      </c>
+      <c r="AJ41" t="str">
+        <f t="shared" si="4"/>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260115.csv</v>
+      </c>
+    </row>
+    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42">
+        <v>2026</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42">
+        <v>20260116</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260116.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260116.csv';</v>
+      </c>
+      <c r="AI42" t="str">
+        <f t="shared" si="3"/>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260116.csv</v>
+      </c>
+      <c r="AJ42" t="str">
+        <f t="shared" si="4"/>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260116.csv</v>
+      </c>
+    </row>
+    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43">
+        <v>2026</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43">
+        <v>20260117</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260117.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260117.csv';</v>
+      </c>
+      <c r="AI43" t="str">
+        <f t="shared" si="3"/>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260117.csv</v>
+      </c>
+      <c r="AJ43" t="str">
+        <f t="shared" si="4"/>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260117.csv</v>
+      </c>
+    </row>
+    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44">
+        <v>2026</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
+        <v>17</v>
+      </c>
+      <c r="E44">
+        <v>20260118</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260118.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260118.csv';</v>
+      </c>
+      <c r="AI44" t="str">
+        <f t="shared" si="3"/>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260118.csv</v>
+      </c>
+      <c r="AJ44" t="str">
+        <f t="shared" si="4"/>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260118.csv</v>
+      </c>
+    </row>
+    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45">
+        <v>2026</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D45" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45">
+        <v>20260119</v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260119.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260119.csv';</v>
+      </c>
+      <c r="AI45" t="str">
+        <f t="shared" si="3"/>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260119.csv</v>
+      </c>
+      <c r="AJ45" t="str">
+        <f t="shared" si="4"/>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260119.csv</v>
+      </c>
+    </row>
+    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>15</v>
+      </c>
+      <c r="B46">
+        <v>2026</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D46" t="s">
+        <v>17</v>
+      </c>
+      <c r="E46">
+        <v>20260120</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260120.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260120.csv';</v>
+      </c>
+      <c r="AI46" t="str">
+        <f t="shared" si="3"/>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260120.csv</v>
+      </c>
+      <c r="AJ46" t="str">
+        <f t="shared" si="4"/>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260120.csv</v>
+      </c>
+    </row>
+    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47">
+        <v>2026</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
+        <v>17</v>
+      </c>
+      <c r="E47">
+        <v>20260121</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260121.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260121.csv';</v>
+      </c>
+      <c r="AI47" t="str">
+        <f t="shared" si="3"/>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260121.csv</v>
+      </c>
+      <c r="AJ47" t="str">
+        <f t="shared" si="4"/>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260121.csv</v>
+      </c>
+    </row>
+    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>15</v>
+      </c>
+      <c r="B48">
+        <v>2026</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
+        <v>17</v>
+      </c>
+      <c r="E48">
+        <v>20260122</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260122.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260122.csv';</v>
+      </c>
+      <c r="AI48" t="str">
+        <f t="shared" si="3"/>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260122.csv</v>
+      </c>
+      <c r="AJ48" t="str">
+        <f t="shared" si="4"/>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260122.csv</v>
+      </c>
+    </row>
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>15</v>
+      </c>
+      <c r="B49">
+        <v>2026</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49" t="s">
+        <v>17</v>
+      </c>
+      <c r="E49">
+        <v>20260123</v>
+      </c>
+      <c r="G49" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260123.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260123.csv';</v>
+      </c>
+      <c r="AI49" t="str">
+        <f t="shared" si="3"/>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260123.csv</v>
+      </c>
+      <c r="AJ49" t="str">
+        <f t="shared" si="4"/>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260123.csv</v>
+      </c>
+    </row>
+    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>15</v>
+      </c>
+      <c r="B50">
+        <v>2026</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
+        <v>17</v>
+      </c>
+      <c r="E50">
+        <v>20260124</v>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260124.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260124.csv';</v>
+      </c>
+      <c r="AI50" t="str">
+        <f t="shared" si="3"/>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260124.csv</v>
+      </c>
+      <c r="AJ50" t="str">
+        <f t="shared" si="4"/>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260124.csv</v>
+      </c>
+    </row>
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51">
+        <v>2026</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
+        <v>17</v>
+      </c>
+      <c r="E51">
+        <v>20260125</v>
+      </c>
+      <c r="G51" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260125.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260125.csv';</v>
+      </c>
+      <c r="AI51" t="str">
+        <f t="shared" si="3"/>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260125.csv</v>
+      </c>
+      <c r="AJ51" t="str">
+        <f t="shared" si="4"/>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260125.csv</v>
+      </c>
+    </row>
+    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>15</v>
+      </c>
+      <c r="B52">
+        <v>2026</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52">
+        <v>20260126</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260126.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260126.csv';</v>
+      </c>
+      <c r="AI52" t="str">
+        <f t="shared" si="3"/>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260126.csv</v>
+      </c>
+      <c r="AJ52" t="str">
+        <f t="shared" si="4"/>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260126.csv</v>
+      </c>
+    </row>
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>15</v>
+      </c>
+      <c r="B53">
+        <v>2026</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
+        <v>17</v>
+      </c>
+      <c r="E53">
+        <v>20260127</v>
+      </c>
+      <c r="G53" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260127.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260127.csv';</v>
+      </c>
+      <c r="AI53" t="str">
+        <f t="shared" si="3"/>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260127.csv</v>
+      </c>
+      <c r="AJ53" t="str">
+        <f t="shared" si="4"/>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260127.csv</v>
+      </c>
+    </row>
+    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>15</v>
+      </c>
+      <c r="B54">
+        <v>2026</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54" t="s">
+        <v>17</v>
+      </c>
+      <c r="E54">
+        <v>20260128</v>
+      </c>
+      <c r="G54" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260128.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260128.csv';</v>
+      </c>
+      <c r="AI54" t="str">
+        <f t="shared" si="3"/>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260128.csv</v>
+      </c>
+      <c r="AJ54" t="str">
+        <f t="shared" si="4"/>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260128.csv</v>
+      </c>
+    </row>
+    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>15</v>
+      </c>
+      <c r="B55">
+        <v>2026</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>17</v>
+      </c>
+      <c r="E55">
+        <v>20260129</v>
+      </c>
+      <c r="G55" t="str">
+        <f t="shared" si="0"/>
+        <v>Start-Sleep -Seconds 3; Invoke-WebRequest -Uri 'https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260129.csv' -OutFile 'D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260129.csv';</v>
+      </c>
+      <c r="AI55" t="str">
+        <f t="shared" si="3"/>
+        <v>https://portal.spp.org/file-browser-api/download/capacity-of-generation-on-outage?path=%2F2026%2F01%2FCapacity-Gen-Outage-20260129.csv</v>
+      </c>
+      <c r="AJ55" t="str">
+        <f t="shared" si="4"/>
+        <v>D:\pub_data_archive\operations\capacity-gen-outage\2026\01\Capacity-Gen-Outage-20260129.csv</v>
       </c>
     </row>
   </sheetData>
@@ -1210,7 +2054,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B220DA0-D201-4B13-B3B1-1493AFCB495F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FBB0445-F974-4AAB-A460-42906AB60650}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="urn:argus-direct-storage:queries"/>
   </ds:schemaRefs>

</xml_diff>